<commit_message>
add functions to find available rooms and choose desired room
</commit_message>
<xml_diff>
--- a/data/raw/rooms.xlsx
+++ b/data/raw/rooms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zech011\win-repos\DSA\dsa-room-booking\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214EACE9-A712-47F9-99E0-B20524BE1C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADD0BC1-5D63-4800-AFB3-FB00D00C2095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>capacity</t>
   </si>
@@ -42,13 +42,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>day</t>
+    <t>available_places</t>
   </si>
   <si>
-    <t>hour</t>
-  </si>
-  <si>
-    <t>available_places</t>
+    <t>date_time</t>
   </si>
 </sst>
 </file>
@@ -56,7 +53,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -87,14 +84,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -375,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,10 +382,10 @@
     <col min="1" max="1" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.1796875" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -406,16 +402,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2.31</v>
       </c>
@@ -432,16 +425,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H2">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2.3199999999999998</v>
       </c>
@@ -458,16 +448,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H3">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2.35</v>
       </c>
@@ -484,16 +471,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H4">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2.4</v>
       </c>
@@ -510,16 +494,13 @@
         <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H5">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2.6</v>
       </c>
@@ -536,16 +517,13 @@
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H6">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2.71</v>
       </c>
@@ -562,16 +540,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H7">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3.01</v>
       </c>
@@ -588,16 +563,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H8">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G8">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3.1</v>
       </c>
@@ -614,16 +586,13 @@
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H9">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3.22</v>
       </c>
@@ -640,16 +609,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H10">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3.33</v>
       </c>
@@ -666,16 +632,13 @@
         <v>0</v>
       </c>
       <c r="F11" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H11">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>3.35</v>
       </c>
@@ -692,16 +655,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H12">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>3.4</v>
       </c>
@@ -718,16 +678,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H13">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G13">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>3.5</v>
       </c>
@@ -744,16 +701,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H14">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G14">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>3.6</v>
       </c>
@@ -770,12 +724,9 @@
         <v>0</v>
       </c>
       <c r="F15" s="3">
-        <v>44562</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="H15">
+        <v>44562.416666666664</v>
+      </c>
+      <c r="G15">
         <v>4</v>
       </c>
     </row>

</xml_diff>